<commit_message>
code added for Dashboard Page
</commit_message>
<xml_diff>
--- a/src/main/java/com/data/SampleExcel.xlsx
+++ b/src/main/java/com/data/SampleExcel.xlsx
@@ -9,11 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
-    <sheet name="Regsitration" sheetId="2" r:id="rId2"/>
+    <sheet name="TestData" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -28,16 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
-  <si>
-    <t>phonenumber</t>
-  </si>
-  <si>
-    <t>age</t>
-  </si>
-  <si>
-    <t>TRUE</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
     <t>Execution</t>
   </si>
@@ -55,6 +46,21 @@
   </si>
   <si>
     <t>HomePageTest</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>madhur_b</t>
+  </si>
+  <si>
+    <t>madhurb</t>
   </si>
 </sst>
 </file>
@@ -387,9 +393,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
-    </sheetView>
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -399,24 +403,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -424,7 +428,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
@@ -437,32 +441,39 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView zoomScale="198" zoomScaleNormal="198" zoomScalePageLayoutView="198" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1">
-        <f>SUM(10+30)</f>
-        <v>40</v>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pushing code for running it from excel flag and tried it from jenkins
</commit_message>
<xml_diff>
--- a/src/main/java/com/data/SampleExcel.xlsx
+++ b/src/main/java/com/data/SampleExcel.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="16">
   <si>
     <t>Execution</t>
   </si>
@@ -61,6 +61,21 @@
   </si>
   <si>
     <t>madhurb</t>
+  </si>
+  <si>
+    <t>DashboardPageTest</t>
+  </si>
+  <si>
+    <t>UpdatePageTest</t>
+  </si>
+  <si>
+    <t>SubmitPageTest</t>
+  </si>
+  <si>
+    <t>ExcelTest</t>
+  </si>
+  <si>
+    <t>CustomerNumber</t>
   </si>
 </sst>
 </file>
@@ -391,17 +406,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -411,8 +430,11 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -423,15 +445,59 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -441,10 +507,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -476,6 +542,17 @@
         <v>10</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>